<commit_message>
improve feature extraction and color folder naming for product scraper
- Enhanced the extraction of product features/specs by searching for all rows in the .pdp-specifications-table and handling <div> elements within value cells, ensuring all feature rows (including those with multiple values) are captured.
- Improved color option folder naming: if the color name is not available from the label, the script now extracts the color name from the first image filename using regex and fallback logic, resulting in more descriptive folder names for color variants.
- Added more robust logging and error handling for image downloads and color extraction.
- Updated code comments and structure for clarity and maintainability.
- These changes improve the completeness and organization of the scraped product data and images.
</commit_message>
<xml_diff>
--- a/extracted_products.xlsx
+++ b/extracted_products.xlsx
@@ -634,12 +634,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Unknown_Color_4</t>
+          <t>Space Blue</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>product_images\Galaxy_S25_Nimbus9_Alto_2_Case\Unknown_Color_4</t>
+          <t>product_images\Galaxy_S25_Nimbus9_Alto_2_Case\Space_Blue</t>
         </is>
       </c>
     </row>

</xml_diff>